<commit_message>
Fix dimes siones file
</commit_message>
<xml_diff>
--- a/dimensiones.xlsx
+++ b/dimensiones.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fc07b1024ec05c40/Documents/Maestría CDD/Ciclo 1/Visualizacion/Proyecto/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marlo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="70" documentId="8_{67F4F375-F5E4-4F86-A025-744F6EFCDAA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD62B025-389B-4CC4-BAE8-BCBA6402B9E3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0FC429-5617-468D-B69C-5227E9A31E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8BF5D375-4565-483A-B1DF-E45BFA2E20BD}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8880" xr2:uid="{8BF5D375-4565-483A-B1DF-E45BFA2E20BD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Departamento " sheetId="1" r:id="rId1"/>
+    <sheet name="Departamento" sheetId="1" r:id="rId1"/>
     <sheet name="Municipio" sheetId="2" r:id="rId2"/>
     <sheet name="Distrito" sheetId="3" r:id="rId3"/>
     <sheet name="M3_Sexo" sheetId="4" r:id="rId4"/>
@@ -39,6 +39,9 @@
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -1598,12 +1601,12 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="31.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1749,12 +1752,12 @@
       <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75">
+    <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1831,12 +1834,12 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75">
+    <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2217,13 +2220,13 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75">
+    <row r="1" spans="1:2">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -4348,13 +4351,13 @@
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75">
+    <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -4391,9 +4394,9 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="31.5">
+    <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -4430,9 +4433,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="31.5">
+    <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -4485,12 +4488,12 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75">
+    <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -4671,9 +4674,9 @@
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="31.5">
+    <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -4710,9 +4713,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="31.5">
+    <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>

</xml_diff>